<commit_message>
feat: Implement ExcelReadingService v1.0.0
Early stage of ExcelReadingService implemented. Need to review error
handling next.
</commit_message>
<xml_diff>
--- a/ExcelReader.BrozDa/ExcelReader.BrozDa/Resources/people-100.xlsx
+++ b/ExcelReader.BrozDa/ExcelReader.BrozDa/Resources/people-100.xlsx
@@ -11,18 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="489">
   <si>
     <t>Index</t>
   </si>
   <si>
+    <t>User Id</t>
+  </si>
+  <si>
     <t>First Name</t>
   </si>
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Sex</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>88F7B33d2bcf9f5</t>
   </si>
   <si>
     <t>Shelby</t>
@@ -31,7 +43,13 @@
     <t>Terrell</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>elijah57@example.net</t>
+  </si>
+  <si>
+    <t>001-084-906-7849x73518</t>
+  </si>
+  <si>
+    <t>f90cD3E76f1A9b9</t>
   </si>
   <si>
     <t>Phillip</t>
@@ -40,7 +58,13 @@
     <t>Summers</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>bethany14@example.com</t>
+  </si>
+  <si>
+    <t>214.112.6044x4913</t>
+  </si>
+  <si>
+    <t>DbeAb8CcdfeFC2c</t>
   </si>
   <si>
     <t>Kristine</t>
@@ -49,559 +73,1420 @@
     <t>Travis</t>
   </si>
   <si>
+    <t>bthompson@example.com</t>
+  </si>
+  <si>
+    <t>277.609.7938</t>
+  </si>
+  <si>
+    <t>A31Bee3c201ef58</t>
+  </si>
+  <si>
     <t>Yesenia</t>
   </si>
   <si>
     <t>Martinez</t>
   </si>
   <si>
+    <t>kaitlinkaiser@example.com</t>
+  </si>
+  <si>
+    <t>584.094.6111</t>
+  </si>
+  <si>
+    <t>1bA7A3dc874da3c</t>
+  </si>
+  <si>
     <t>Lori</t>
   </si>
   <si>
     <t>Todd</t>
   </si>
   <si>
+    <t>buchananmanuel@example.net</t>
+  </si>
+  <si>
+    <t>689-207-3558x7233</t>
+  </si>
+  <si>
+    <t>bfDD7CDEF5D865B</t>
+  </si>
+  <si>
     <t>Erin</t>
   </si>
   <si>
     <t>Day</t>
   </si>
   <si>
+    <t>tconner@example.org</t>
+  </si>
+  <si>
+    <t>001-171-649-9856x5553</t>
+  </si>
+  <si>
+    <t>bE9EEf34cB72AF7</t>
+  </si>
+  <si>
     <t>Katherine</t>
   </si>
   <si>
     <t>Buck</t>
   </si>
   <si>
+    <t>conniecowan@example.com</t>
+  </si>
+  <si>
+    <t>+1-773-151-6685x49162</t>
+  </si>
+  <si>
+    <t>2EFC6A4e77FaEaC</t>
+  </si>
+  <si>
     <t>Ricardo</t>
   </si>
   <si>
     <t>Hinton</t>
   </si>
   <si>
+    <t>wyattbishop@example.com</t>
+  </si>
+  <si>
+    <t>001-447-699-7998x88612</t>
+  </si>
+  <si>
+    <t>baDcC4DeefD8dEB</t>
+  </si>
+  <si>
     <t>Dave</t>
   </si>
   <si>
     <t>Farrell</t>
   </si>
   <si>
+    <t>nmccann@example.net</t>
+  </si>
+  <si>
+    <t>603-428-2429x27392</t>
+  </si>
+  <si>
+    <t>8e4FB470FE19bF0</t>
+  </si>
+  <si>
     <t>Isaiah</t>
   </si>
   <si>
     <t>Downs</t>
   </si>
   <si>
+    <t>virginiaterrell@example.org</t>
+  </si>
+  <si>
+    <t>+1-511-372-1544x8206</t>
+  </si>
+  <si>
+    <t>BF0BbA03C29Bb3b</t>
+  </si>
+  <si>
     <t>Sheila</t>
   </si>
   <si>
     <t>Ross</t>
   </si>
   <si>
+    <t>huangcathy@example.com</t>
+  </si>
+  <si>
+    <t>895.881.4746</t>
+  </si>
+  <si>
+    <t>F738c69fB34E62E</t>
+  </si>
+  <si>
     <t>Stacy</t>
   </si>
   <si>
     <t>Newton</t>
   </si>
   <si>
+    <t>rayleroy@example.org</t>
+  </si>
+  <si>
+    <t>710.673.3213x80335</t>
+  </si>
+  <si>
+    <t>C03fDADdAadAdCe</t>
+  </si>
+  <si>
     <t>Mandy</t>
   </si>
   <si>
     <t>Blake</t>
   </si>
   <si>
+    <t>jefferynoble@example.org</t>
+  </si>
+  <si>
+    <t>(992)466-1305x4947</t>
+  </si>
+  <si>
+    <t>b759b74BD1dE80d</t>
+  </si>
+  <si>
     <t>Bridget</t>
   </si>
   <si>
     <t>Nash</t>
   </si>
   <si>
+    <t>mercedes44@example.com</t>
+  </si>
+  <si>
+    <t>(216)627-8359</t>
+  </si>
+  <si>
+    <t>1F0B7D65A00DAF9</t>
+  </si>
+  <si>
     <t>Crystal</t>
   </si>
   <si>
     <t>Farmer</t>
   </si>
   <si>
+    <t>pmiranda@example.org</t>
+  </si>
+  <si>
+    <t>+1-024-377-5391</t>
+  </si>
+  <si>
+    <t>50Bb061cB30B461</t>
+  </si>
+  <si>
     <t>Thomas</t>
   </si>
   <si>
     <t>Knight</t>
   </si>
   <si>
+    <t>braunpriscilla@example.net</t>
+  </si>
+  <si>
+    <t>+1-360-880-0766</t>
+  </si>
+  <si>
+    <t>D6dbA5308fEC4BC</t>
+  </si>
+  <si>
     <t>Maurice</t>
   </si>
   <si>
     <t>Rangel</t>
   </si>
   <si>
+    <t>sheenabanks@example.com</t>
+  </si>
+  <si>
+    <t>(246)187-4969</t>
+  </si>
+  <si>
+    <t>311D775990f066d</t>
+  </si>
+  <si>
     <t>Frank</t>
   </si>
   <si>
     <t>Meadows</t>
   </si>
   <si>
+    <t>gbrewer@example.org</t>
+  </si>
+  <si>
+    <t>429.965.3902x4447</t>
+  </si>
+  <si>
+    <t>7F7E1BAcb0C9AFf</t>
+  </si>
+  <si>
     <t>Alvin</t>
   </si>
   <si>
     <t>Paul</t>
   </si>
   <si>
+    <t>gilbertdonaldson@example.com</t>
+  </si>
+  <si>
+    <t>219.436.0887x07551</t>
+  </si>
+  <si>
+    <t>88473e15D5c3cD0</t>
+  </si>
+  <si>
     <t>Jared</t>
   </si>
   <si>
     <t>Mitchell</t>
   </si>
   <si>
+    <t>jcortez@example.com</t>
+  </si>
+  <si>
+    <t>+1-958-849-6781</t>
+  </si>
+  <si>
+    <t>b31D271F8c200AB</t>
+  </si>
+  <si>
     <t>Jacqueline</t>
   </si>
   <si>
     <t>Norton</t>
   </si>
   <si>
+    <t>carias@example.net</t>
+  </si>
+  <si>
+    <t>819.309.7679x59173</t>
+  </si>
+  <si>
+    <t>42F4BdA841aBadC</t>
+  </si>
+  <si>
     <t>Colleen</t>
   </si>
   <si>
     <t>Hatfield</t>
   </si>
   <si>
+    <t>fknox@example.org</t>
+  </si>
+  <si>
+    <t>638.584.1090</t>
+  </si>
+  <si>
+    <t>cBbBcA0FCA3C4Bc</t>
+  </si>
+  <si>
     <t>Randy</t>
   </si>
   <si>
     <t>Barnes</t>
   </si>
   <si>
+    <t>huangbill@example.org</t>
+  </si>
+  <si>
+    <t>001-960-629-7164x67214</t>
+  </si>
+  <si>
+    <t>f1f89173353aD90</t>
+  </si>
+  <si>
     <t>Janice</t>
   </si>
   <si>
     <t>Rhodes</t>
   </si>
   <si>
+    <t>juarezdominique@example.net</t>
+  </si>
+  <si>
+    <t>001-249-314-9742x6996</t>
+  </si>
+  <si>
+    <t>c5B09fb33e8bA0A</t>
+  </si>
+  <si>
     <t>Alfred</t>
   </si>
   <si>
     <t>Mcneil</t>
   </si>
   <si>
+    <t>cassandramorris@example.com</t>
+  </si>
+  <si>
+    <t>(468)276-9509x53058</t>
+  </si>
+  <si>
+    <t>c9F2282C40BEC1E</t>
+  </si>
+  <si>
     <t>Sean</t>
   </si>
   <si>
     <t>Levine</t>
   </si>
   <si>
+    <t>sallymiller@example.net</t>
+  </si>
+  <si>
+    <t>9c1bc7EC53Fb7cE</t>
+  </si>
+  <si>
     <t>Louis</t>
   </si>
   <si>
     <t>Payne</t>
   </si>
   <si>
+    <t>bsullivan@example.net</t>
+  </si>
+  <si>
+    <t>ddEc50e2A2e3a2B</t>
+  </si>
+  <si>
     <t>Brittney</t>
   </si>
   <si>
     <t>Vega</t>
   </si>
   <si>
+    <t>ayalajose@example.net</t>
+  </si>
+  <si>
+    <t>945-739-8686</t>
+  </si>
+  <si>
+    <t>66F096D36Ebae11</t>
+  </si>
+  <si>
     <t>Judy</t>
   </si>
   <si>
     <t>Buckley</t>
   </si>
   <si>
+    <t>irosales@example.net</t>
+  </si>
+  <si>
+    <t>001-654-208-1241x52830</t>
+  </si>
+  <si>
+    <t>F0fE2faAd78F8b5</t>
+  </si>
+  <si>
     <t>Norman</t>
   </si>
   <si>
     <t>Weber</t>
   </si>
   <si>
+    <t>mconrad@example.com</t>
+  </si>
+  <si>
+    <t>223.002.0429</t>
+  </si>
+  <si>
+    <t>5d2feAfbdCAA6B5</t>
+  </si>
+  <si>
     <t>Camacho</t>
   </si>
   <si>
+    <t>jimblake@example.org</t>
+  </si>
+  <si>
+    <t>001-536-544-3367</t>
+  </si>
+  <si>
+    <t>cDa5F303fCd6dEa</t>
+  </si>
+  <si>
     <t>Gallagher</t>
   </si>
   <si>
+    <t>nsampson@example.net</t>
+  </si>
+  <si>
+    <t>(247)762-8934</t>
+  </si>
+  <si>
+    <t>8Ef7DBfcaB02b6B</t>
+  </si>
+  <si>
     <t>Bonnie</t>
   </si>
   <si>
     <t>Andrews</t>
   </si>
   <si>
+    <t>caitlin24@example.net</t>
+  </si>
+  <si>
+    <t>+1-253-987-2776x9161</t>
+  </si>
+  <si>
+    <t>6Dec5b5542F8ed8</t>
+  </si>
+  <si>
     <t>Brandon</t>
   </si>
   <si>
     <t>Schmidt</t>
   </si>
   <si>
+    <t>mconley@example.net</t>
+  </si>
+  <si>
+    <t>+1-386-673-1465x006</t>
+  </si>
+  <si>
+    <t>3Fb8a7f68e12784</t>
+  </si>
+  <si>
     <t>Jackson</t>
   </si>
   <si>
     <t>Sparks</t>
   </si>
   <si>
+    <t>reynoldsdarryl@example.net</t>
+  </si>
+  <si>
+    <t>(137)908-3129x65035</t>
+  </si>
+  <si>
+    <t>035eff50B9A0F24</t>
+  </si>
+  <si>
     <t>Melody</t>
   </si>
   <si>
     <t>Cook</t>
   </si>
   <si>
+    <t>jeannovak@example.org</t>
+  </si>
+  <si>
+    <t>(826)792-7381</t>
+  </si>
+  <si>
+    <t>aa614aAE4B7Cf0C</t>
+  </si>
+  <si>
     <t>Leonard</t>
   </si>
   <si>
     <t>Hurst</t>
   </si>
   <si>
+    <t>clinton78@example.org</t>
+  </si>
+  <si>
+    <t>941-038-0427x38800</t>
+  </si>
+  <si>
+    <t>ACcde95AAe3e6cC</t>
+  </si>
+  <si>
     <t>Gene</t>
   </si>
   <si>
     <t>Rich</t>
   </si>
   <si>
+    <t>luisdeleon@example.org</t>
+  </si>
+  <si>
+    <t>+1-356-818-6604x89537</t>
+  </si>
+  <si>
+    <t>b6a35de5CB6fc25</t>
+  </si>
+  <si>
     <t>Cynthia</t>
   </si>
   <si>
     <t>Wiggins</t>
   </si>
   <si>
+    <t>rosariodave@example.org</t>
+  </si>
+  <si>
+    <t>(110)858-2437x70190</t>
+  </si>
+  <si>
+    <t>e92A191E345fA3A</t>
+  </si>
+  <si>
     <t>Tanya</t>
   </si>
   <si>
     <t>Mckinney</t>
   </si>
   <si>
+    <t>vickihouston@example.com</t>
+  </si>
+  <si>
+    <t>(830)774-9002x086</t>
+  </si>
+  <si>
+    <t>7D0AcBF6CCac3fd</t>
+  </si>
+  <si>
     <t>Matthew</t>
   </si>
   <si>
     <t>Stone</t>
   </si>
   <si>
+    <t>evelyn31@example.org</t>
+  </si>
+  <si>
+    <t>952-381-6360</t>
+  </si>
+  <si>
+    <t>CEFA7BBCef013AE</t>
+  </si>
+  <si>
     <t>Kirk</t>
   </si>
   <si>
     <t>Walsh</t>
   </si>
   <si>
+    <t>stephenfuller@example.org</t>
+  </si>
+  <si>
+    <t>001-826-496-5529x8661</t>
+  </si>
+  <si>
+    <t>9edBC94aE7cA22a</t>
+  </si>
+  <si>
     <t>Willie</t>
   </si>
   <si>
     <t>Vang</t>
   </si>
   <si>
+    <t>haleymathews@example.net</t>
+  </si>
+  <si>
+    <t>741.168.6854x067</t>
+  </si>
+  <si>
+    <t>fFe7BAA737aDbe2</t>
+  </si>
+  <si>
     <t>Miguel</t>
   </si>
   <si>
     <t>Hill</t>
   </si>
   <si>
+    <t>tyrone56@example.org</t>
+  </si>
+  <si>
+    <t>5F2f3fAca8B0946</t>
+  </si>
+  <si>
     <t>Darren</t>
   </si>
   <si>
+    <t>lhernandez@example.com</t>
+  </si>
+  <si>
+    <t>(975)799-4261</t>
+  </si>
+  <si>
+    <t>6bFcfc3cc1BC6B4</t>
+  </si>
+  <si>
     <t>Haley</t>
   </si>
   <si>
     <t>Pugh</t>
   </si>
   <si>
+    <t>molly03@example.org</t>
+  </si>
+  <si>
+    <t>(746)182-6137x2453</t>
+  </si>
+  <si>
+    <t>f3BD2cBF7eEb6df</t>
+  </si>
+  <si>
     <t>Danielle</t>
   </si>
   <si>
     <t>Estrada</t>
   </si>
   <si>
+    <t>jvang@example.org</t>
+  </si>
+  <si>
+    <t>(890)374-9518x772</t>
+  </si>
+  <si>
+    <t>Ee4eB129dC7913A</t>
+  </si>
+  <si>
     <t>Becky</t>
   </si>
   <si>
     <t>Brady</t>
   </si>
   <si>
+    <t>erikmueller@example.org</t>
+  </si>
+  <si>
+    <t>(390)002-0863</t>
+  </si>
+  <si>
+    <t>dBCEf340C3657Eb</t>
+  </si>
+  <si>
     <t>Caitlyn</t>
   </si>
   <si>
     <t>Frey</t>
   </si>
   <si>
+    <t>rivasdominique@example.org</t>
+  </si>
+  <si>
+    <t>805-021-3965x46344</t>
+  </si>
+  <si>
+    <t>E47FB71DD9ACCd9</t>
+  </si>
+  <si>
     <t>Joshua</t>
   </si>
   <si>
     <t>Sweeney</t>
   </si>
   <si>
+    <t>daisymcgee@example.net</t>
+  </si>
+  <si>
+    <t>875.994.2100x535</t>
+  </si>
+  <si>
+    <t>eA3fDd79BE9f0E7</t>
+  </si>
+  <si>
     <t>Heidi</t>
   </si>
   <si>
     <t>Escobar</t>
   </si>
   <si>
+    <t>staffordtravis@example.net</t>
+  </si>
+  <si>
+    <t>601-155-3065x1131</t>
+  </si>
+  <si>
+    <t>aF0eE4547Bc025c</t>
+  </si>
+  <si>
     <t>Brian</t>
   </si>
   <si>
     <t>Oconnell</t>
   </si>
   <si>
+    <t>saralong@example.net</t>
+  </si>
+  <si>
+    <t>952-283-1423x733</t>
+  </si>
+  <si>
+    <t>9F5DeD7aD228F5a</t>
+  </si>
+  <si>
     <t>Beverly</t>
   </si>
   <si>
     <t>Esparza</t>
   </si>
   <si>
+    <t>iphelps@example.net</t>
+  </si>
+  <si>
+    <t>+1-327-578-8754x6771</t>
+  </si>
+  <si>
+    <t>D3Fa0220dDE4d36</t>
+  </si>
+  <si>
     <t>Nathaniel</t>
   </si>
   <si>
     <t>Rivas</t>
   </si>
   <si>
+    <t>roberto29@example.com</t>
+  </si>
+  <si>
+    <t>(655)887-2040x37888</t>
+  </si>
+  <si>
+    <t>60FdBFd5e7BE8fF</t>
+  </si>
+  <si>
     <t>Debra</t>
   </si>
   <si>
+    <t>yolanda07@example.org</t>
+  </si>
+  <si>
+    <t>001-731-525-8400x52593</t>
+  </si>
+  <si>
+    <t>D8bF5Ab2b98caff</t>
+  </si>
+  <si>
     <t>Mackenzie</t>
   </si>
   <si>
     <t>Rocha</t>
   </si>
   <si>
+    <t>abbottyvette@example.net</t>
+  </si>
+  <si>
+    <t>CD8d33aA25bc8BB</t>
+  </si>
+  <si>
     <t>Courtney</t>
   </si>
   <si>
     <t>Watkins</t>
   </si>
   <si>
+    <t>ochang@example.org</t>
+  </si>
+  <si>
+    <t>210.683.2761x5883</t>
+  </si>
+  <si>
+    <t>Fac3BfFf0A3d03c</t>
+  </si>
+  <si>
     <t>Fred</t>
   </si>
   <si>
     <t>Olsen</t>
   </si>
   <si>
+    <t>amyanderson@example.com</t>
+  </si>
+  <si>
+    <t>497-774-3053</t>
+  </si>
+  <si>
+    <t>e552D7ddafe1FFb</t>
+  </si>
+  <si>
     <t>Ryan</t>
   </si>
   <si>
     <t>Nelson</t>
   </si>
   <si>
+    <t>qnorman@example.org</t>
+  </si>
+  <si>
+    <t>956.330.2951</t>
+  </si>
+  <si>
+    <t>0f8deedb629A5f6</t>
+  </si>
+  <si>
     <t>Grace</t>
   </si>
   <si>
     <t>Phelps</t>
   </si>
   <si>
+    <t>clarkeangela@example.net</t>
+  </si>
+  <si>
+    <t>(034)867-8827x6777</t>
+  </si>
+  <si>
+    <t>bB9e49E506F65ed</t>
+  </si>
+  <si>
     <t>Shari</t>
   </si>
   <si>
     <t>Daugherty</t>
   </si>
   <si>
+    <t>kalvarado@example.org</t>
+  </si>
+  <si>
+    <t>001-951-655-4798x6124</t>
+  </si>
+  <si>
+    <t>Ed724605A403D91</t>
+  </si>
+  <si>
     <t>Kelli</t>
   </si>
   <si>
     <t>Garner</t>
   </si>
   <si>
+    <t>jodyvincent@example.org</t>
+  </si>
+  <si>
+    <t>995.000.4213x0982</t>
+  </si>
+  <si>
+    <t>0aBE5ACb18E0c10</t>
+  </si>
+  <si>
     <t>Jackie</t>
   </si>
   <si>
     <t>Bennett</t>
   </si>
   <si>
+    <t>hutchinsonkirk@example.com</t>
+  </si>
+  <si>
+    <t>001-740-937-0846x0087</t>
+  </si>
+  <si>
+    <t>5D2cb63CaAF53f6</t>
+  </si>
+  <si>
     <t>Leslie</t>
   </si>
   <si>
     <t>Conway</t>
   </si>
   <si>
+    <t>floreschristina@example.org</t>
+  </si>
+  <si>
+    <t>795.782.4384x555</t>
+  </si>
+  <si>
+    <t>Ee6974f90eeCe18</t>
+  </si>
+  <si>
     <t>Harold</t>
   </si>
   <si>
     <t>Barnett</t>
   </si>
   <si>
+    <t>nathan65@example.org</t>
+  </si>
+  <si>
+    <t>+1-026-265-6392</t>
+  </si>
+  <si>
+    <t>cEf02C076afa07f</t>
+  </si>
+  <si>
     <t>Larry</t>
   </si>
   <si>
     <t>Harper</t>
   </si>
   <si>
+    <t>maria32@example.org</t>
+  </si>
+  <si>
+    <t>+1-244-630-3792x4121</t>
+  </si>
+  <si>
+    <t>9Df5Ba591bF3EFf</t>
+  </si>
+  <si>
     <t>Mike</t>
   </si>
   <si>
     <t>Ward</t>
   </si>
   <si>
+    <t>imccullough@example.com</t>
+  </si>
+  <si>
+    <t>116-729-5046</t>
+  </si>
+  <si>
+    <t>3faB1CBfEFBDdD4</t>
+  </si>
+  <si>
     <t>Rubio</t>
   </si>
   <si>
+    <t>corey92@example.com</t>
+  </si>
+  <si>
+    <t>593.976.2528</t>
+  </si>
+  <si>
+    <t>Ebcefdf75eCb0a9</t>
+  </si>
+  <si>
     <t>Pineda</t>
   </si>
   <si>
+    <t>daltoncalvin@example.net</t>
+  </si>
+  <si>
+    <t>(035)961-5060x9182</t>
+  </si>
+  <si>
+    <t>e75e5DBfcb68887</t>
+  </si>
+  <si>
     <t>Sandra</t>
   </si>
   <si>
     <t>Wu</t>
   </si>
   <si>
+    <t>ubanks@example.com</t>
+  </si>
+  <si>
+    <t>+1-096-606-6454x067</t>
+  </si>
+  <si>
+    <t>6a53a8D41dDF6de</t>
+  </si>
+  <si>
     <t>Benton</t>
   </si>
   <si>
+    <t>lopezdebbie@example.org</t>
+  </si>
+  <si>
+    <t>+1-695-557-9948x485</t>
+  </si>
+  <si>
+    <t>F0d3bD1aaf9E3Bc</t>
+  </si>
+  <si>
     <t>Tamara</t>
   </si>
   <si>
     <t>Hull</t>
   </si>
   <si>
+    <t>meagan39@example.net</t>
+  </si>
+  <si>
+    <t>017.665.3744x7944</t>
+  </si>
+  <si>
+    <t>5bC87340799FBD0</t>
+  </si>
+  <si>
     <t>Jean</t>
   </si>
   <si>
     <t>Ritter</t>
   </si>
   <si>
+    <t>kristina76@example.com</t>
+  </si>
+  <si>
+    <t>(954)060-1066</t>
+  </si>
+  <si>
+    <t>dBfA17Aaf16b4ab</t>
+  </si>
+  <si>
     <t>Veronica</t>
   </si>
   <si>
     <t>Briggs</t>
   </si>
   <si>
+    <t>weissbridget@example.com</t>
+  </si>
+  <si>
+    <t>+1-521-589-2387x48490</t>
+  </si>
+  <si>
+    <t>c935b7Eb6FA0B0F</t>
+  </si>
+  <si>
     <t>Kim</t>
   </si>
   <si>
+    <t>wpetersen@example.org</t>
+  </si>
+  <si>
+    <t>b3e15e65Ca2CcBf</t>
+  </si>
+  <si>
     <t>Tina</t>
   </si>
   <si>
     <t>Cunningham</t>
   </si>
   <si>
+    <t>wongmary@example.org</t>
+  </si>
+  <si>
+    <t>079-907-5051</t>
+  </si>
+  <si>
+    <t>dade3452F0c32FD</t>
+  </si>
+  <si>
     <t>Jonathon</t>
   </si>
   <si>
     <t>Atkinson</t>
   </si>
   <si>
+    <t>gailfrench@example.net</t>
+  </si>
+  <si>
+    <t>874-037-2032x932</t>
+  </si>
+  <si>
+    <t>AdEd6cfD85DeC46</t>
+  </si>
+  <si>
     <t>Jermaine</t>
   </si>
   <si>
     <t>Reid</t>
   </si>
   <si>
+    <t>vpaul@example.com</t>
+  </si>
+  <si>
+    <t>(742)214-8691</t>
+  </si>
+  <si>
+    <t>DAf111987098ae4</t>
+  </si>
+  <si>
     <t>Regina</t>
   </si>
   <si>
     <t>Stevens</t>
   </si>
   <si>
+    <t>xpoole@example.net</t>
+  </si>
+  <si>
+    <t>891-359-2684</t>
+  </si>
+  <si>
+    <t>6e6a5b885F6496d</t>
+  </si>
+  <si>
     <t>Terrence</t>
   </si>
   <si>
     <t>Huff</t>
   </si>
   <si>
+    <t>cassandra80@example.org</t>
+  </si>
+  <si>
+    <t>221.800.6408x5416</t>
+  </si>
+  <si>
+    <t>12DCb4ED8E01D5C</t>
+  </si>
+  <si>
     <t>Tyler</t>
   </si>
   <si>
     <t>Foley</t>
   </si>
   <si>
+    <t>johnathan72@example.org</t>
+  </si>
+  <si>
+    <t>001-386-469-3075x8030</t>
+  </si>
+  <si>
+    <t>E1cB5cA8CA7CC0a</t>
+  </si>
+  <si>
     <t>Andrew</t>
   </si>
   <si>
     <t>Waters</t>
   </si>
   <si>
+    <t>nhall@example.net</t>
+  </si>
+  <si>
+    <t>+1-376-865-2765x3351</t>
+  </si>
+  <si>
+    <t>AedDfaE8Cf49F07</t>
+  </si>
+  <si>
     <t>Reginald</t>
   </si>
   <si>
     <t>Stephenson</t>
   </si>
   <si>
+    <t>erikaball@example.net</t>
+  </si>
+  <si>
+    <t>+1-832-500-6044x475</t>
+  </si>
+  <si>
+    <t>bff9853aFAeF772</t>
+  </si>
+  <si>
     <t>Douglas</t>
   </si>
   <si>
     <t>Reese</t>
   </si>
   <si>
+    <t>nixonvanessa@example.net</t>
+  </si>
+  <si>
+    <t>001-834-660-8312x9864</t>
+  </si>
+  <si>
+    <t>E883773cA5219Be</t>
+  </si>
+  <si>
     <t>Helen</t>
   </si>
   <si>
     <t>Williamson</t>
   </si>
   <si>
+    <t>melvin08@example.net</t>
+  </si>
+  <si>
+    <t>001-377-726-4229</t>
+  </si>
+  <si>
+    <t>CB19EafEbBfF9eC</t>
+  </si>
+  <si>
     <t>Mario</t>
   </si>
   <si>
     <t>Vaughn</t>
   </si>
   <si>
+    <t>oblake@example.com</t>
+  </si>
+  <si>
+    <t>160-144-5039x12276</t>
+  </si>
+  <si>
+    <t>5834700fbEd2771</t>
+  </si>
+  <si>
     <t>Chelsea</t>
   </si>
   <si>
     <t>Dickson</t>
   </si>
   <si>
+    <t>johnnyhendricks@example.net</t>
+  </si>
+  <si>
+    <t>001-698-651-0138x18588</t>
+  </si>
+  <si>
+    <t>2b0Ab1Dc9E01D7E</t>
+  </si>
+  <si>
     <t>Dustin</t>
   </si>
   <si>
     <t>Bailey</t>
   </si>
   <si>
+    <t>pbarron@example.net</t>
+  </si>
+  <si>
+    <t>+1-965-621-1157x345</t>
+  </si>
+  <si>
+    <t>3f3a3D89ad042Dd</t>
+  </si>
+  <si>
     <t>Harry</t>
   </si>
   <si>
     <t>Medina</t>
   </si>
   <si>
+    <t>olsenmalik@example.net</t>
+  </si>
+  <si>
+    <t>+1-451-099-5805</t>
+  </si>
+  <si>
+    <t>9425E2F38C408ef</t>
+  </si>
+  <si>
     <t>Kathy</t>
   </si>
   <si>
     <t>Haney</t>
   </si>
   <si>
+    <t>teresa37@example.com</t>
+  </si>
+  <si>
+    <t>(164)105-8456</t>
+  </si>
+  <si>
+    <t>F0aeC9c2759F3C6</t>
+  </si>
+  <si>
     <t>Alison</t>
   </si>
   <si>
     <t>Nixon</t>
   </si>
   <si>
+    <t>zmiles@example.net</t>
+  </si>
+  <si>
+    <t>d6EA619A7C4aA95</t>
+  </si>
+  <si>
     <t>Jamie</t>
   </si>
   <si>
     <t>Hardy</t>
   </si>
   <si>
+    <t>sheenadouglas@example.com</t>
+  </si>
+  <si>
+    <t>(900)803-9295x11533</t>
+  </si>
+  <si>
+    <t>2A33E7Cad1bb0F5</t>
+  </si>
+  <si>
     <t>Cox</t>
   </si>
   <si>
+    <t>evan90@example.org</t>
+  </si>
+  <si>
+    <t>(626)520-5080x3511</t>
+  </si>
+  <si>
+    <t>d181FFB7d3E68bb</t>
+  </si>
+  <si>
     <t>Xavier</t>
   </si>
   <si>
     <t>Cole</t>
   </si>
   <si>
+    <t>nicolas90@example.org</t>
+  </si>
+  <si>
+    <t>feaBf8dAE0C0d6F</t>
+  </si>
+  <si>
     <t>Dillon</t>
   </si>
   <si>
     <t>Guzman</t>
   </si>
   <si>
+    <t>angelanavarro@example.net</t>
+  </si>
+  <si>
+    <t>971-992-4521</t>
+  </si>
+  <si>
+    <t>5eFda7caAeB260E</t>
+  </si>
+  <si>
     <t>Dennis</t>
   </si>
   <si>
+    <t>bmartin@example.org</t>
+  </si>
+  <si>
+    <t>001-095-524-2112x257</t>
+  </si>
+  <si>
+    <t>CCbFce93d3720bE</t>
+  </si>
+  <si>
     <t>Steve</t>
   </si>
   <si>
     <t>Patterson</t>
   </si>
   <si>
+    <t>latasha46@example.net</t>
+  </si>
+  <si>
+    <t>001-865-478-5157</t>
+  </si>
+  <si>
+    <t>2fEc528aFAF0b69</t>
+  </si>
+  <si>
     <t>Wesley</t>
   </si>
   <si>
     <t>Bray</t>
   </si>
   <si>
+    <t>regina11@example.org</t>
+  </si>
+  <si>
+    <t>995-542-3004x76800</t>
+  </si>
+  <si>
+    <t>Adc7ad9B6e4A1Fe</t>
+  </si>
+  <si>
     <t>Summer</t>
   </si>
   <si>
+    <t>alexiscantrell@example.org</t>
+  </si>
+  <si>
+    <t>001-273-685-6932x092</t>
+  </si>
+  <si>
+    <t>b8D0aD3490FC7e1</t>
+  </si>
+  <si>
     <t>Mariah</t>
   </si>
   <si>
     <t>Bernard</t>
+  </si>
+  <si>
+    <t>pcopeland@example.org</t>
+  </si>
+  <si>
+    <t>(341)594-6554x44657</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -629,11 +1514,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -852,7 +1740,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="14.75"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
+    <col customWidth="1" min="5" max="5" width="25.63"/>
+    <col customWidth="1" min="6" max="6" width="27.5"/>
+    <col customWidth="1" min="7" max="7" width="14.13"/>
+    <col customWidth="1" min="8" max="8" width="47.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -868,19 +1760,37 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2">
+        <v>16736.0</v>
       </c>
     </row>
     <row r="3">
@@ -888,13 +1798,22 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3736.0</v>
       </c>
     </row>
     <row r="4">
@@ -902,13 +1821,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2">
+        <v>33787.0</v>
       </c>
     </row>
     <row r="5">
@@ -916,13 +1844,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
+        <v>42950.0</v>
       </c>
     </row>
     <row r="6">
@@ -930,13 +1867,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2">
+        <v>14215.0</v>
       </c>
     </row>
     <row r="7">
@@ -944,13 +1890,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>42305.0</v>
       </c>
     </row>
     <row r="8">
@@ -958,13 +1913,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2">
+        <v>32530.0</v>
       </c>
     </row>
     <row r="9">
@@ -972,13 +1936,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8852.0</v>
       </c>
     </row>
     <row r="10">
@@ -986,13 +1959,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43379.0</v>
       </c>
     </row>
     <row r="11">
@@ -1000,13 +1982,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2">
+        <v>23640.0</v>
       </c>
     </row>
     <row r="12">
@@ -1014,13 +2005,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="2">
+        <v>39527.0</v>
       </c>
     </row>
     <row r="13">
@@ -1028,13 +2028,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="2">
+        <v>29514.0</v>
       </c>
     </row>
     <row r="14">
@@ -1042,13 +2051,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="2">
+        <v>39424.0</v>
       </c>
     </row>
     <row r="15">
@@ -1056,13 +2074,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>74</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="2">
+        <v>38166.0</v>
       </c>
     </row>
     <row r="16">
@@ -1070,13 +2097,22 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>79</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="2">
+        <v>33672.0</v>
       </c>
     </row>
     <row r="17">
@@ -1084,13 +2120,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="2">
+        <v>38766.0</v>
       </c>
     </row>
     <row r="18">
@@ -1098,13 +2143,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>89</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="2">
+        <v>38219.0</v>
       </c>
     </row>
     <row r="19">
@@ -1112,13 +2166,22 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="2">
+        <v>39707.0</v>
       </c>
     </row>
     <row r="20">
@@ -1126,13 +2189,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>99</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="2">
+        <v>18030.0</v>
       </c>
     </row>
     <row r="21">
@@ -1140,13 +2212,22 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>104</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7689.0</v>
       </c>
     </row>
     <row r="22">
@@ -1154,13 +2235,22 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="2">
+        <v>19276.0</v>
       </c>
     </row>
     <row r="23">
@@ -1168,13 +2258,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="2">
+        <v>18185.0</v>
       </c>
     </row>
     <row r="24">
@@ -1182,13 +2281,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>6</v>
+        <v>119</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="2">
+        <v>17531.0</v>
       </c>
     </row>
     <row r="25">
@@ -1196,13 +2304,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>124</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="2">
+        <v>36465.0</v>
       </c>
     </row>
     <row r="26">
@@ -1210,13 +2327,22 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>129</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="2">
+        <v>34117.0</v>
       </c>
     </row>
     <row r="27">
@@ -1224,13 +2350,22 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>6</v>
+        <v>134</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4.915828504E9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>40460.0</v>
       </c>
     </row>
     <row r="28">
@@ -1238,13 +2373,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>6</v>
+        <v>138</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="1">
+        <v>6.232695307E9</v>
+      </c>
+      <c r="G28" s="2">
+        <v>5873.0</v>
       </c>
     </row>
     <row r="29">
@@ -1252,13 +2396,22 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>9</v>
+        <v>142</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" s="2">
+        <v>11993.0</v>
       </c>
     </row>
     <row r="30">
@@ -1266,13 +2419,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>6</v>
+        <v>147</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" s="2">
+        <v>23220.0</v>
       </c>
     </row>
     <row r="31">
@@ -1280,13 +2442,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>151</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>6</v>
+        <v>152</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G31" s="2">
+        <v>20961.0</v>
       </c>
     </row>
     <row r="32">
@@ -1294,13 +2465,22 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>9</v>
+        <v>156</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="2">
+        <v>24204.0</v>
       </c>
     </row>
     <row r="33">
@@ -1308,13 +2488,22 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
+        <v>159</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>6</v>
+        <v>160</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="2">
+        <v>36216.0</v>
       </c>
     </row>
     <row r="34">
@@ -1322,13 +2511,22 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="2">
+        <v>19714.0</v>
       </c>
     </row>
     <row r="35">
@@ -1336,13 +2534,22 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>170</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="2">
+        <v>11455.0</v>
       </c>
     </row>
     <row r="36">
@@ -1350,13 +2557,22 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>9</v>
+        <v>175</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="2">
+        <v>29543.0</v>
       </c>
     </row>
     <row r="37">
@@ -1364,13 +2580,22 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>6</v>
+        <v>180</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G37" s="2">
+        <v>23187.0</v>
       </c>
     </row>
     <row r="38">
@@ -1378,13 +2603,22 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>183</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>184</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>6</v>
+        <v>185</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G38" s="2">
+        <v>13952.0</v>
       </c>
     </row>
     <row r="39">
@@ -1392,13 +2626,22 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>190</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G39" s="2">
+        <v>17036.0</v>
       </c>
     </row>
     <row r="40">
@@ -1406,13 +2649,22 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>195</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G40" s="2">
+        <v>30708.0</v>
       </c>
     </row>
     <row r="41">
@@ -1420,13 +2672,22 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>200</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G41" s="2">
+        <v>37692.0</v>
       </c>
     </row>
     <row r="42">
@@ -1434,13 +2695,22 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>203</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>85</v>
+        <v>204</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>205</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G42" s="2">
+        <v>42970.0</v>
       </c>
     </row>
     <row r="43">
@@ -1448,13 +2718,22 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>9</v>
+        <v>210</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G43" s="2">
+        <v>39911.0</v>
       </c>
     </row>
     <row r="44">
@@ -1462,13 +2741,22 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>89</v>
+        <v>214</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9</v>
+        <v>215</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G44" s="2">
+        <v>28523.0</v>
       </c>
     </row>
     <row r="45">
@@ -1476,13 +2764,22 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
+        <v>219</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>9</v>
+        <v>220</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F45" s="1">
+        <v>5.247842945E9</v>
+      </c>
+      <c r="G45" s="2">
+        <v>11196.0</v>
       </c>
     </row>
     <row r="46">
@@ -1490,13 +2787,22 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>222</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>69</v>
+        <v>223</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>6</v>
+        <v>165</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G46" s="2">
+        <v>35707.0</v>
       </c>
     </row>
     <row r="47">
@@ -1504,13 +2810,22 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>94</v>
+        <v>227</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>9</v>
+        <v>228</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G47" s="2">
+        <v>29480.0</v>
       </c>
     </row>
     <row r="48">
@@ -1518,13 +2833,22 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>231</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>96</v>
+        <v>232</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>9</v>
+        <v>233</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G48" s="2">
+        <v>11148.0</v>
       </c>
     </row>
     <row r="49">
@@ -1532,13 +2856,22 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>6</v>
+        <v>238</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G49" s="2">
+        <v>20998.0</v>
       </c>
     </row>
     <row r="50">
@@ -1546,13 +2879,22 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>241</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>100</v>
+        <v>242</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>6</v>
+        <v>243</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G50" s="2">
+        <v>24863.0</v>
       </c>
     </row>
     <row r="51">
@@ -1560,13 +2902,22 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>246</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>102</v>
+        <v>247</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>6</v>
+        <v>248</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G51" s="2">
+        <v>19933.0</v>
       </c>
     </row>
     <row r="52">
@@ -1574,13 +2925,22 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>104</v>
+        <v>252</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>9</v>
+        <v>253</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G52" s="2">
+        <v>11591.0</v>
       </c>
     </row>
     <row r="53">
@@ -1588,13 +2948,22 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>256</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>106</v>
+        <v>257</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>9</v>
+        <v>258</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" s="2">
+        <v>4314.0</v>
       </c>
     </row>
     <row r="54">
@@ -1602,13 +2971,22 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>261</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>108</v>
+        <v>262</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>9</v>
+        <v>263</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G54" s="2">
+        <v>11301.0</v>
       </c>
     </row>
     <row r="55">
@@ -1616,13 +2994,22 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>109</v>
+        <v>266</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>110</v>
+        <v>267</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>9</v>
+        <v>268</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G55" s="2">
+        <v>3244.0</v>
       </c>
     </row>
     <row r="56">
@@ -1630,13 +3017,22 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>271</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>272</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>138</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G56" s="2">
+        <v>10094.0</v>
       </c>
     </row>
     <row r="57">
@@ -1644,13 +3040,22 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>275</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>113</v>
+        <v>276</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>9</v>
+        <v>277</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F57" s="1">
+        <v>4.225525458E9</v>
+      </c>
+      <c r="G57" s="2">
+        <v>29515.0</v>
       </c>
     </row>
     <row r="58">
@@ -1658,13 +3063,22 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>115</v>
+        <v>280</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>9</v>
+        <v>281</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G58" s="2">
+        <v>37962.0</v>
       </c>
     </row>
     <row r="59">
@@ -1672,13 +3086,22 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>284</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>285</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>9</v>
+        <v>286</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G59" s="2">
+        <v>3753.0</v>
       </c>
     </row>
     <row r="60">
@@ -1686,13 +3109,22 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>119</v>
+        <v>290</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>9</v>
+        <v>291</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G60" s="2">
+        <v>8889.0</v>
       </c>
     </row>
     <row r="61">
@@ -1700,13 +3132,22 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>120</v>
+        <v>294</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>121</v>
+        <v>295</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>6</v>
+        <v>296</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G61" s="2">
+        <v>3576.0</v>
       </c>
     </row>
     <row r="62">
@@ -1714,13 +3155,22 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>299</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>6</v>
+        <v>301</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G62" s="2">
+        <v>16400.0</v>
       </c>
     </row>
     <row r="63">
@@ -1728,13 +3178,22 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>124</v>
+        <v>304</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>125</v>
+        <v>305</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>6</v>
+        <v>306</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G63" s="2">
+        <v>40195.0</v>
       </c>
     </row>
     <row r="64">
@@ -1742,13 +3201,22 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>126</v>
+        <v>309</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>127</v>
+        <v>310</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>6</v>
+        <v>311</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G64" s="2">
+        <v>5794.0</v>
       </c>
     </row>
     <row r="65">
@@ -1756,13 +3224,22 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>314</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>129</v>
+        <v>315</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>9</v>
+        <v>316</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G65" s="2">
+        <v>30626.0</v>
       </c>
     </row>
     <row r="66">
@@ -1770,13 +3247,22 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>319</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>131</v>
+        <v>320</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>9</v>
+        <v>321</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G66" s="2">
+        <v>15780.0</v>
       </c>
     </row>
     <row r="67">
@@ -1784,13 +3270,22 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>324</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>133</v>
+        <v>325</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>6</v>
+        <v>326</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G67" s="2">
+        <v>44321.0</v>
       </c>
     </row>
     <row r="68">
@@ -1798,13 +3293,22 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>134</v>
+        <v>329</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>135</v>
+        <v>330</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>9</v>
+        <v>331</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G68" s="2">
+        <v>24785.0</v>
       </c>
     </row>
     <row r="69">
@@ -1812,13 +3316,22 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>60</v>
+        <v>334</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>9</v>
+        <v>335</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G69" s="2">
+        <v>21908.0</v>
       </c>
     </row>
     <row r="70">
@@ -1826,13 +3339,22 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>40</v>
+        <v>338</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>6</v>
+        <v>339</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G70" s="2">
+        <v>9566.0</v>
       </c>
     </row>
     <row r="71">
@@ -1840,13 +3362,22 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>138</v>
+        <v>342</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>139</v>
+        <v>343</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>6</v>
+        <v>344</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G71" s="2">
+        <v>9250.0</v>
       </c>
     </row>
     <row r="72">
@@ -1854,13 +3385,22 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>118</v>
+        <v>347</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>140</v>
+        <v>290</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>6</v>
+        <v>348</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G72" s="2">
+        <v>44110.0</v>
       </c>
     </row>
     <row r="73">
@@ -1868,13 +3408,22 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>141</v>
+        <v>351</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>142</v>
+        <v>352</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>6</v>
+        <v>353</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G73" s="2">
+        <v>12085.0</v>
       </c>
     </row>
     <row r="74">
@@ -1882,13 +3431,22 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>143</v>
+        <v>356</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>144</v>
+        <v>357</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>9</v>
+        <v>358</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G74" s="2">
+        <v>31265.0</v>
       </c>
     </row>
     <row r="75">
@@ -1896,13 +3454,22 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>145</v>
+        <v>361</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>146</v>
+        <v>362</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>9</v>
+        <v>363</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G75" s="2">
+        <v>27188.0</v>
       </c>
     </row>
     <row r="76">
@@ -1910,13 +3477,22 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>147</v>
+        <v>366</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>69</v>
+        <v>367</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="F76" s="1">
+        <v>7.677125383E9</v>
+      </c>
+      <c r="G76" s="2">
+        <v>33192.0</v>
       </c>
     </row>
     <row r="77">
@@ -1924,13 +3500,22 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>148</v>
+        <v>369</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>149</v>
+        <v>370</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>6</v>
+        <v>371</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G77" s="2">
+        <v>20788.0</v>
       </c>
     </row>
     <row r="78">
@@ -1938,13 +3523,22 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>150</v>
+        <v>374</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>151</v>
+        <v>375</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>6</v>
+        <v>376</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G78" s="2">
+        <v>40743.0</v>
       </c>
     </row>
     <row r="79">
@@ -1952,13 +3546,22 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>152</v>
+        <v>379</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>153</v>
+        <v>380</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>9</v>
+        <v>381</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G79" s="2">
+        <v>27259.0</v>
       </c>
     </row>
     <row r="80">
@@ -1966,13 +3569,22 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>154</v>
+        <v>384</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>155</v>
+        <v>385</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>6</v>
+        <v>386</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G80" s="2">
+        <v>40875.0</v>
       </c>
     </row>
     <row r="81">
@@ -1980,13 +3592,22 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>156</v>
+        <v>389</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>157</v>
+        <v>390</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>6</v>
+        <v>391</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G81" s="2">
+        <v>16129.0</v>
       </c>
     </row>
     <row r="82">
@@ -1994,13 +3615,22 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>158</v>
+        <v>394</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>159</v>
+        <v>395</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>9</v>
+        <v>396</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G82" s="2">
+        <v>3185.0</v>
       </c>
     </row>
     <row r="83">
@@ -2008,13 +3638,22 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>160</v>
+        <v>399</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>161</v>
+        <v>400</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>6</v>
+        <v>401</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G83" s="2">
+        <v>17667.0</v>
       </c>
     </row>
     <row r="84">
@@ -2022,13 +3661,22 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>162</v>
+        <v>404</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>163</v>
+        <v>405</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>6</v>
+        <v>406</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G84" s="2">
+        <v>40217.0</v>
       </c>
     </row>
     <row r="85">
@@ -2036,13 +3684,22 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>164</v>
+        <v>409</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>165</v>
+        <v>410</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>9</v>
+        <v>411</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G85" s="2">
+        <v>22596.0</v>
       </c>
     </row>
     <row r="86">
@@ -2050,13 +3707,22 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>166</v>
+        <v>414</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>167</v>
+        <v>415</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>9</v>
+        <v>416</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G86" s="2">
+        <v>4241.0</v>
       </c>
     </row>
     <row r="87">
@@ -2064,13 +3730,22 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>168</v>
+        <v>419</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>169</v>
+        <v>420</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>6</v>
+        <v>421</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G87" s="2">
+        <v>33062.0</v>
       </c>
     </row>
     <row r="88">
@@ -2078,13 +3753,22 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>424</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>171</v>
+        <v>425</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>6</v>
+        <v>426</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G88" s="2">
+        <v>21318.0</v>
       </c>
     </row>
     <row r="89">
@@ -2092,13 +3776,22 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>172</v>
+        <v>429</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>173</v>
+        <v>430</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>6</v>
+        <v>431</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G89" s="2">
+        <v>3157.0</v>
       </c>
     </row>
     <row r="90">
@@ -2106,13 +3799,22 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>174</v>
+        <v>434</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>175</v>
+        <v>435</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>9</v>
+        <v>436</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G90" s="2">
+        <v>17403.0</v>
       </c>
     </row>
     <row r="91">
@@ -2120,13 +3822,22 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>176</v>
+        <v>439</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>177</v>
+        <v>440</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>9</v>
+        <v>441</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G91" s="2">
+        <v>20334.0</v>
       </c>
     </row>
     <row r="92">
@@ -2134,13 +3845,22 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>179</v>
+        <v>445</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>9</v>
+        <v>446</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F92" s="1">
+        <v>3.506680871E9</v>
+      </c>
+      <c r="G92" s="2">
+        <v>15167.0</v>
       </c>
     </row>
     <row r="93">
@@ -2148,13 +3868,22 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>180</v>
+        <v>448</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>181</v>
+        <v>449</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>9</v>
+        <v>450</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G93" s="2">
+        <v>34532.0</v>
       </c>
     </row>
     <row r="94">
@@ -2162,13 +3891,22 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>74</v>
+        <v>453</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>9</v>
+        <v>454</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G94" s="2">
+        <v>27240.0</v>
       </c>
     </row>
     <row r="95">
@@ -2176,13 +3914,22 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>183</v>
+        <v>457</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>184</v>
+        <v>458</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>6</v>
+        <v>459</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F95" s="1">
+        <v>8.164259975E9</v>
+      </c>
+      <c r="G95" s="2">
+        <v>14213.0</v>
       </c>
     </row>
     <row r="96">
@@ -2190,13 +3937,22 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>185</v>
+        <v>461</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>186</v>
+        <v>462</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>9</v>
+        <v>463</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G96" s="2">
+        <v>15432.0</v>
       </c>
     </row>
     <row r="97">
@@ -2204,13 +3960,22 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>187</v>
+        <v>466</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>51</v>
+        <v>467</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>9</v>
+        <v>119</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G97" s="2">
+        <v>19935.0</v>
       </c>
     </row>
     <row r="98">
@@ -2218,13 +3983,22 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>188</v>
+        <v>470</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>189</v>
+        <v>471</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>9</v>
+        <v>472</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G98" s="2">
+        <v>11808.0</v>
       </c>
     </row>
     <row r="99">
@@ -2232,13 +4006,22 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>190</v>
+        <v>475</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>191</v>
+        <v>476</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>6</v>
+        <v>477</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G99" s="2">
+        <v>34696.0</v>
       </c>
     </row>
     <row r="100">
@@ -2246,13 +4029,22 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>192</v>
+        <v>480</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>106</v>
+        <v>481</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>9</v>
+        <v>258</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G100" s="2">
+        <v>41011.0</v>
       </c>
     </row>
     <row r="101">
@@ -2260,13 +4052,22 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>193</v>
+        <v>484</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>194</v>
+        <v>485</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>6</v>
+        <v>486</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="G101" s="2">
+        <v>42689.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>